<commit_message>
Bulk upload refernce file update
</commit_message>
<xml_diff>
--- a/api/public/files/members/Upload_Members_reference_file.xlsx
+++ b/api/public/files/members/Upload_Members_reference_file.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="14295" windowHeight="4620" tabRatio="441"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="14292" windowHeight="4620" tabRatio="441" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Member Info" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="59">
   <si>
     <t>First Name</t>
   </si>
@@ -191,6 +191,31 @@
   <si>
     <t>demo@demo.com</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Fields marked </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>red</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> are mandatory..</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -200,7 +225,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
     <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,8 +254,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -243,8 +282,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -304,6 +349,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -312,7 +366,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -365,6 +419,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -670,47 +728,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q334"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" style="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.140625" style="14" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.5703125" style="14" customWidth="1"/>
-    <col min="11" max="11" width="23.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="14" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="19.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.42578125" style="14" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.5703125" style="14" customWidth="1"/>
-    <col min="18" max="18" width="20.140625" style="14" customWidth="1"/>
-    <col min="19" max="19" width="22.140625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="27.109375" style="14" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5546875" style="14" customWidth="1"/>
+    <col min="11" max="11" width="23.109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.109375" style="14" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="19.5546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.44140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.44140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5546875" style="14" customWidth="1"/>
+    <col min="18" max="18" width="20.109375" style="14" customWidth="1"/>
+    <col min="19" max="19" width="22.109375" style="14" customWidth="1"/>
     <col min="20" max="20" width="16" style="14" customWidth="1"/>
-    <col min="21" max="21" width="16.140625" style="14" customWidth="1"/>
-    <col min="22" max="22" width="20.7109375" style="14" customWidth="1"/>
-    <col min="23" max="23" width="17.140625" style="14" customWidth="1"/>
-    <col min="24" max="25" width="9.140625" style="14"/>
-    <col min="26" max="26" width="14.7109375" style="14" customWidth="1"/>
+    <col min="21" max="21" width="16.109375" style="14" customWidth="1"/>
+    <col min="22" max="22" width="20.6640625" style="14" customWidth="1"/>
+    <col min="23" max="23" width="17.109375" style="14" customWidth="1"/>
+    <col min="24" max="25" width="9.109375" style="14"/>
+    <col min="26" max="26" width="14.6640625" style="14" customWidth="1"/>
     <col min="27" max="27" width="32" style="14" customWidth="1"/>
-    <col min="28" max="28" width="18.140625" style="14" customWidth="1"/>
-    <col min="29" max="16384" width="9.140625" style="14"/>
+    <col min="28" max="28" width="18.109375" style="14" customWidth="1"/>
+    <col min="29" max="16384" width="9.109375" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="21" t="s">
@@ -725,10 +783,10 @@
       <c r="F1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="23" t="s">
         <v>13</v>
       </c>
       <c r="I1" s="21" t="s">
@@ -757,7 +815,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>55</v>
       </c>
@@ -807,7 +865,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="D3" s="9"/>
@@ -821,7 +879,7 @@
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="D4" s="9"/>
@@ -835,7 +893,7 @@
       <c r="O4" s="6"/>
       <c r="P4" s="6"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="D5" s="9"/>
@@ -850,7 +908,7 @@
       <c r="O5" s="6"/>
       <c r="P5" s="6"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="D6" s="9"/>
@@ -864,7 +922,7 @@
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="D7" s="9"/>
@@ -878,7 +936,7 @@
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="D8" s="9"/>
@@ -892,7 +950,7 @@
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="D9" s="9"/>
@@ -906,7 +964,7 @@
       <c r="O9" s="6"/>
       <c r="P9" s="6"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="D10" s="9"/>
@@ -920,7 +978,7 @@
       <c r="O10" s="6"/>
       <c r="P10" s="6"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="D11" s="9"/>
@@ -934,7 +992,7 @@
       <c r="O11" s="6"/>
       <c r="P11" s="6"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="D12" s="9"/>
@@ -948,7 +1006,7 @@
       <c r="O12" s="6"/>
       <c r="P12" s="6"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="D13" s="9"/>
@@ -962,7 +1020,7 @@
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="D14" s="9"/>
@@ -976,7 +1034,7 @@
       <c r="O14" s="6"/>
       <c r="P14" s="6"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="D15" s="9"/>
@@ -990,7 +1048,7 @@
       <c r="O15" s="6"/>
       <c r="P15" s="6"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="D16" s="9"/>
@@ -1004,7 +1062,7 @@
       <c r="O16" s="6"/>
       <c r="P16" s="6"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
       <c r="D17" s="9"/>
@@ -1018,7 +1076,7 @@
       <c r="O17" s="6"/>
       <c r="P17" s="6"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="D18" s="9"/>
@@ -1032,7 +1090,7 @@
       <c r="O18" s="6"/>
       <c r="P18" s="6"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" s="6"/>
       <c r="D19" s="9"/>
@@ -1046,7 +1104,7 @@
       <c r="O19" s="6"/>
       <c r="P19" s="6"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="D20" s="9"/>
@@ -1060,7 +1118,7 @@
       <c r="O20" s="6"/>
       <c r="P20" s="6"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="D21" s="9"/>
@@ -1074,7 +1132,7 @@
       <c r="O21" s="6"/>
       <c r="P21" s="6"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="D22" s="9"/>
@@ -1088,7 +1146,7 @@
       <c r="O22" s="6"/>
       <c r="P22" s="6"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="D23" s="9"/>
@@ -1103,7 +1161,7 @@
       <c r="O23" s="6"/>
       <c r="P23" s="6"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
       <c r="B24" s="6"/>
       <c r="D24" s="9"/>
@@ -1118,7 +1176,7 @@
       <c r="O24" s="6"/>
       <c r="P24" s="6"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
       <c r="B25" s="6"/>
       <c r="D25" s="9"/>
@@ -1132,7 +1190,7 @@
       <c r="O25" s="6"/>
       <c r="P25" s="6"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
       <c r="B26" s="6"/>
       <c r="D26" s="9"/>
@@ -1146,7 +1204,7 @@
       <c r="O26" s="6"/>
       <c r="P26" s="6"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27" s="20"/>
       <c r="B27" s="20"/>
       <c r="D27" s="9"/>
@@ -1161,7 +1219,7 @@
       <c r="O27" s="6"/>
       <c r="P27" s="6"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="6"/>
       <c r="B28" s="6"/>
       <c r="D28" s="9"/>
@@ -1175,7 +1233,7 @@
       <c r="O28" s="6"/>
       <c r="P28" s="6"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="6"/>
       <c r="B29" s="6"/>
       <c r="D29" s="9"/>
@@ -1189,7 +1247,7 @@
       <c r="O29" s="6"/>
       <c r="P29" s="6"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
       <c r="D30" s="9"/>
@@ -1203,7 +1261,7 @@
       <c r="O30" s="6"/>
       <c r="P30" s="6"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
       <c r="D31" s="9"/>
@@ -1218,7 +1276,7 @@
       <c r="O31" s="6"/>
       <c r="P31" s="6"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="D32" s="9"/>
@@ -1232,7 +1290,7 @@
       <c r="O32" s="6"/>
       <c r="P32" s="6"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
       <c r="D33" s="9"/>
@@ -1246,7 +1304,7 @@
       <c r="O33" s="6"/>
       <c r="P33" s="6"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="6"/>
       <c r="B34" s="6"/>
       <c r="D34" s="9"/>
@@ -1260,7 +1318,7 @@
       <c r="O34" s="6"/>
       <c r="P34" s="6"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="6"/>
       <c r="B35" s="6"/>
       <c r="D35" s="9"/>
@@ -1274,7 +1332,7 @@
       <c r="O35" s="6"/>
       <c r="P35" s="6"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" s="6"/>
       <c r="B36" s="6"/>
       <c r="D36" s="9"/>
@@ -1288,7 +1346,7 @@
       <c r="O36" s="6"/>
       <c r="P36" s="6"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" s="20"/>
       <c r="B37" s="20"/>
       <c r="D37" s="9"/>
@@ -1303,7 +1361,7 @@
       <c r="O37" s="6"/>
       <c r="P37" s="6"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="D38" s="9"/>
@@ -1317,7 +1375,7 @@
       <c r="O38" s="6"/>
       <c r="P38" s="6"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="D39" s="9"/>
@@ -1331,7 +1389,7 @@
       <c r="O39" s="6"/>
       <c r="P39" s="6"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
       <c r="D40" s="9"/>
@@ -1345,7 +1403,7 @@
       <c r="O40" s="6"/>
       <c r="P40" s="6"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" s="6"/>
       <c r="B41" s="6"/>
       <c r="D41" s="9"/>
@@ -1359,7 +1417,7 @@
       <c r="O41" s="6"/>
       <c r="P41" s="6"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42" s="6"/>
       <c r="B42" s="6"/>
       <c r="D42" s="9"/>
@@ -1373,7 +1431,7 @@
       <c r="O42" s="6"/>
       <c r="P42" s="6"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="D43" s="9"/>
@@ -1387,7 +1445,7 @@
       <c r="O43" s="6"/>
       <c r="P43" s="6"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
       <c r="D44" s="9"/>
@@ -1401,7 +1459,7 @@
       <c r="O44" s="6"/>
       <c r="P44" s="6"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="6"/>
       <c r="B45" s="6"/>
       <c r="D45" s="9"/>
@@ -1415,7 +1473,7 @@
       <c r="O45" s="6"/>
       <c r="P45" s="6"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46" s="6"/>
       <c r="B46" s="6"/>
       <c r="D46" s="9"/>
@@ -1429,7 +1487,7 @@
       <c r="O46" s="6"/>
       <c r="P46" s="6"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
       <c r="D47" s="9"/>
@@ -1443,7 +1501,7 @@
       <c r="O47" s="6"/>
       <c r="P47" s="6"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" s="6"/>
       <c r="B48" s="6"/>
       <c r="D48" s="9"/>
@@ -1457,7 +1515,7 @@
       <c r="O48" s="6"/>
       <c r="P48" s="6"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
       <c r="D49" s="9"/>
@@ -1472,7 +1530,7 @@
       <c r="O49" s="6"/>
       <c r="P49" s="6"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" s="6"/>
       <c r="B50" s="6"/>
       <c r="D50" s="9"/>
@@ -1486,7 +1544,7 @@
       <c r="O50" s="6"/>
       <c r="P50" s="6"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" s="6"/>
       <c r="B51" s="6"/>
       <c r="D51" s="9"/>
@@ -1500,7 +1558,7 @@
       <c r="O51" s="6"/>
       <c r="P51" s="6"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
       <c r="D52" s="9"/>
@@ -1515,7 +1573,7 @@
       <c r="O52" s="6"/>
       <c r="P52" s="6"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" s="6"/>
       <c r="B53" s="6"/>
       <c r="D53" s="9"/>
@@ -1530,7 +1588,7 @@
       <c r="O53" s="6"/>
       <c r="P53" s="6"/>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
       <c r="D54" s="9"/>
@@ -1544,7 +1602,7 @@
       <c r="O54" s="6"/>
       <c r="P54" s="6"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" s="6"/>
       <c r="B55" s="6"/>
       <c r="D55" s="9"/>
@@ -1558,7 +1616,7 @@
       <c r="O55" s="6"/>
       <c r="P55" s="6"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56" s="6"/>
       <c r="B56" s="6"/>
       <c r="D56" s="9"/>
@@ -1572,7 +1630,7 @@
       <c r="O56" s="6"/>
       <c r="P56" s="6"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57" s="6"/>
       <c r="B57" s="6"/>
       <c r="D57" s="9"/>
@@ -1586,7 +1644,7 @@
       <c r="O57" s="6"/>
       <c r="P57" s="6"/>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
       <c r="D58" s="9"/>
@@ -1600,7 +1658,7 @@
       <c r="O58" s="6"/>
       <c r="P58" s="6"/>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59" s="6"/>
       <c r="B59" s="6"/>
       <c r="D59" s="9"/>
@@ -1614,7 +1672,7 @@
       <c r="O59" s="6"/>
       <c r="P59" s="6"/>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A60" s="6"/>
       <c r="B60" s="6"/>
       <c r="D60" s="9"/>
@@ -1628,7 +1686,7 @@
       <c r="O60" s="6"/>
       <c r="P60" s="6"/>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61" s="6"/>
       <c r="B61" s="6"/>
       <c r="D61" s="9"/>
@@ -1642,7 +1700,7 @@
       <c r="O61" s="6"/>
       <c r="P61" s="6"/>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A62" s="8"/>
       <c r="B62" s="8"/>
       <c r="D62" s="9"/>
@@ -1657,7 +1715,7 @@
       <c r="O62" s="6"/>
       <c r="P62" s="6"/>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63" s="6"/>
       <c r="B63" s="6"/>
       <c r="D63" s="9"/>
@@ -1671,7 +1729,7 @@
       <c r="O63" s="6"/>
       <c r="P63" s="6"/>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A64" s="6"/>
       <c r="B64" s="6"/>
       <c r="D64" s="9"/>
@@ -1685,7 +1743,7 @@
       <c r="O64" s="6"/>
       <c r="P64" s="6"/>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65" s="8"/>
       <c r="B65" s="8"/>
       <c r="D65" s="9"/>
@@ -1699,7 +1757,7 @@
       <c r="O65" s="6"/>
       <c r="P65" s="6"/>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66" s="6"/>
       <c r="B66" s="6"/>
       <c r="D66" s="9"/>
@@ -1713,7 +1771,7 @@
       <c r="O66" s="6"/>
       <c r="P66" s="6"/>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67" s="6"/>
       <c r="B67" s="6"/>
       <c r="D67" s="9"/>
@@ -1728,7 +1786,7 @@
       <c r="O67" s="6"/>
       <c r="P67" s="6"/>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A68" s="6"/>
       <c r="B68" s="6"/>
       <c r="D68" s="9"/>
@@ -1742,7 +1800,7 @@
       <c r="O68" s="6"/>
       <c r="P68" s="6"/>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A69" s="6"/>
       <c r="B69" s="6"/>
       <c r="D69" s="9"/>
@@ -1756,7 +1814,7 @@
       <c r="O69" s="6"/>
       <c r="P69" s="6"/>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A70" s="8"/>
       <c r="B70" s="8"/>
       <c r="D70" s="9"/>
@@ -1771,7 +1829,7 @@
       <c r="O70" s="6"/>
       <c r="P70" s="6"/>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A71" s="6"/>
       <c r="B71" s="6"/>
       <c r="D71" s="9"/>
@@ -1785,7 +1843,7 @@
       <c r="O71" s="6"/>
       <c r="P71" s="6"/>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A72" s="6"/>
       <c r="B72" s="6"/>
       <c r="D72" s="9"/>
@@ -1799,7 +1857,7 @@
       <c r="O72" s="6"/>
       <c r="P72" s="6"/>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A73" s="6"/>
       <c r="B73" s="6"/>
       <c r="D73" s="9"/>
@@ -1813,7 +1871,7 @@
       <c r="O73" s="6"/>
       <c r="P73" s="6"/>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A74" s="6"/>
       <c r="B74" s="6"/>
       <c r="D74" s="9"/>
@@ -1827,7 +1885,7 @@
       <c r="O74" s="6"/>
       <c r="P74" s="6"/>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A75" s="6"/>
       <c r="B75" s="6"/>
       <c r="D75" s="9"/>
@@ -1841,7 +1899,7 @@
       <c r="O75" s="6"/>
       <c r="P75" s="6"/>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A76" s="6"/>
       <c r="B76" s="6"/>
       <c r="D76" s="9"/>
@@ -1855,7 +1913,7 @@
       <c r="O76" s="6"/>
       <c r="P76" s="6"/>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A77" s="6"/>
       <c r="B77" s="6"/>
       <c r="D77" s="9"/>
@@ -1869,7 +1927,7 @@
       <c r="O77" s="6"/>
       <c r="P77" s="6"/>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A78" s="6"/>
       <c r="B78" s="6"/>
       <c r="D78" s="9"/>
@@ -1884,7 +1942,7 @@
       <c r="O78" s="6"/>
       <c r="P78" s="6"/>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A79" s="8"/>
       <c r="B79" s="8"/>
       <c r="D79" s="9"/>
@@ -1898,7 +1956,7 @@
       <c r="O79" s="6"/>
       <c r="P79" s="6"/>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A80" s="8"/>
       <c r="B80" s="8"/>
       <c r="D80" s="9"/>
@@ -1912,7 +1970,7 @@
       <c r="O80" s="6"/>
       <c r="P80" s="6"/>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A81" s="6"/>
       <c r="B81" s="6"/>
       <c r="D81" s="9"/>
@@ -1926,7 +1984,7 @@
       <c r="O81" s="6"/>
       <c r="P81" s="6"/>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A82" s="6"/>
       <c r="B82" s="6"/>
       <c r="D82" s="9"/>
@@ -1940,7 +1998,7 @@
       <c r="O82" s="6"/>
       <c r="P82" s="6"/>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A83" s="6"/>
       <c r="B83" s="6"/>
       <c r="D83" s="9"/>
@@ -1954,7 +2012,7 @@
       <c r="O83" s="6"/>
       <c r="P83" s="6"/>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A84" s="6"/>
       <c r="B84" s="6"/>
       <c r="D84" s="9"/>
@@ -1968,7 +2026,7 @@
       <c r="O84" s="6"/>
       <c r="P84" s="6"/>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A85" s="6"/>
       <c r="B85" s="6"/>
       <c r="D85" s="9"/>
@@ -1982,7 +2040,7 @@
       <c r="O85" s="6"/>
       <c r="P85" s="6"/>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A86" s="6"/>
       <c r="B86" s="6"/>
       <c r="D86" s="9"/>
@@ -1996,7 +2054,7 @@
       <c r="O86" s="6"/>
       <c r="P86" s="6"/>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A87" s="6"/>
       <c r="B87" s="6"/>
       <c r="D87" s="9"/>
@@ -2010,7 +2068,7 @@
       <c r="O87" s="6"/>
       <c r="P87" s="6"/>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A88" s="6"/>
       <c r="B88" s="6"/>
       <c r="D88" s="9"/>
@@ -2024,7 +2082,7 @@
       <c r="O88" s="8"/>
       <c r="P88" s="6"/>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A89" s="6"/>
       <c r="B89" s="6"/>
       <c r="D89" s="9"/>
@@ -2038,7 +2096,7 @@
       <c r="O89" s="6"/>
       <c r="P89" s="6"/>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A90" s="6"/>
       <c r="B90" s="6"/>
       <c r="D90" s="9"/>
@@ -2052,7 +2110,7 @@
       <c r="O90" s="6"/>
       <c r="P90" s="6"/>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A91" s="6"/>
       <c r="B91" s="6"/>
       <c r="D91" s="9"/>
@@ -2066,7 +2124,7 @@
       <c r="O91" s="6"/>
       <c r="P91" s="6"/>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A92" s="6"/>
       <c r="B92" s="6"/>
       <c r="D92" s="9"/>
@@ -2080,7 +2138,7 @@
       <c r="O92" s="8"/>
       <c r="P92" s="6"/>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A93" s="6"/>
       <c r="B93" s="6"/>
       <c r="D93" s="9"/>
@@ -2094,7 +2152,7 @@
       <c r="O93" s="6"/>
       <c r="P93" s="6"/>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A94" s="6"/>
       <c r="B94" s="6"/>
       <c r="D94" s="9"/>
@@ -2108,7 +2166,7 @@
       <c r="O94" s="6"/>
       <c r="P94" s="6"/>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A95" s="6"/>
       <c r="B95" s="6"/>
       <c r="D95" s="9"/>
@@ -2122,7 +2180,7 @@
       <c r="O95" s="6"/>
       <c r="P95" s="6"/>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A96" s="6"/>
       <c r="B96" s="6"/>
       <c r="D96" s="9"/>
@@ -2136,7 +2194,7 @@
       <c r="O96" s="6"/>
       <c r="P96" s="6"/>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A97" s="6"/>
       <c r="B97" s="6"/>
       <c r="D97" s="9"/>
@@ -2150,7 +2208,7 @@
       <c r="O97" s="6"/>
       <c r="P97" s="15"/>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A98" s="6"/>
       <c r="B98" s="6"/>
       <c r="D98" s="9"/>
@@ -2164,7 +2222,7 @@
       <c r="O98" s="6"/>
       <c r="P98" s="15"/>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A99" s="6"/>
       <c r="B99" s="6"/>
       <c r="D99" s="9"/>
@@ -2178,7 +2236,7 @@
       <c r="O99" s="6"/>
       <c r="P99" s="6"/>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A100" s="6"/>
       <c r="B100" s="6"/>
       <c r="D100" s="9"/>
@@ -2192,7 +2250,7 @@
       <c r="O100" s="6"/>
       <c r="P100" s="6"/>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A101" s="6"/>
       <c r="B101" s="6"/>
       <c r="D101" s="9"/>
@@ -2206,7 +2264,7 @@
       <c r="O101" s="6"/>
       <c r="P101" s="15"/>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A102" s="6"/>
       <c r="B102" s="6"/>
       <c r="D102" s="9"/>
@@ -2220,7 +2278,7 @@
       <c r="O102" s="6"/>
       <c r="P102" s="6"/>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A103" s="6"/>
       <c r="B103" s="6"/>
       <c r="D103" s="9"/>
@@ -2234,7 +2292,7 @@
       <c r="O103" s="6"/>
       <c r="P103" s="15"/>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A104" s="6"/>
       <c r="B104" s="6"/>
       <c r="D104" s="9"/>
@@ -2248,7 +2306,7 @@
       <c r="O104" s="6"/>
       <c r="P104" s="6"/>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A105" s="6"/>
       <c r="B105" s="6"/>
       <c r="D105" s="9"/>
@@ -2262,7 +2320,7 @@
       <c r="O105" s="6"/>
       <c r="P105" s="15"/>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A106" s="6"/>
       <c r="B106" s="6"/>
       <c r="D106" s="9"/>
@@ -2276,7 +2334,7 @@
       <c r="O106" s="6"/>
       <c r="P106" s="6"/>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A107" s="6"/>
       <c r="B107" s="6"/>
       <c r="D107" s="9"/>
@@ -2290,7 +2348,7 @@
       <c r="O107" s="6"/>
       <c r="P107" s="6"/>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A108" s="8"/>
       <c r="B108" s="8"/>
       <c r="D108" s="9"/>
@@ -2304,7 +2362,7 @@
       <c r="O108" s="6"/>
       <c r="P108" s="6"/>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A109" s="8"/>
       <c r="B109" s="8"/>
       <c r="D109" s="9"/>
@@ -2318,7 +2376,7 @@
       <c r="O109" s="6"/>
       <c r="P109" s="10"/>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A110" s="6"/>
       <c r="B110" s="6"/>
       <c r="D110" s="9"/>
@@ -2332,7 +2390,7 @@
       <c r="O110" s="6"/>
       <c r="P110" s="10"/>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A111" s="6"/>
       <c r="B111" s="6"/>
       <c r="D111" s="9"/>
@@ -2346,7 +2404,7 @@
       <c r="O111" s="6"/>
       <c r="P111" s="6"/>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A112" s="8"/>
       <c r="B112" s="8"/>
       <c r="D112" s="9"/>
@@ -2360,7 +2418,7 @@
       <c r="O112" s="6"/>
       <c r="P112" s="10"/>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A113" s="6"/>
       <c r="B113" s="6"/>
       <c r="D113" s="9"/>
@@ -2374,7 +2432,7 @@
       <c r="O113" s="6"/>
       <c r="P113" s="6"/>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A114" s="6"/>
       <c r="B114" s="6"/>
       <c r="D114" s="9"/>
@@ -2388,7 +2446,7 @@
       <c r="O114" s="6"/>
       <c r="P114" s="6"/>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A115" s="6"/>
       <c r="B115" s="6"/>
       <c r="D115" s="9"/>
@@ -2402,7 +2460,7 @@
       <c r="O115" s="6"/>
       <c r="P115" s="6"/>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A116" s="6"/>
       <c r="B116" s="6"/>
       <c r="D116" s="9"/>
@@ -2416,7 +2474,7 @@
       <c r="O116" s="6"/>
       <c r="P116" s="6"/>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A117" s="6"/>
       <c r="B117" s="6"/>
       <c r="D117" s="9"/>
@@ -2430,7 +2488,7 @@
       <c r="O117" s="6"/>
       <c r="P117" s="15"/>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A118" s="8"/>
       <c r="B118" s="8"/>
       <c r="D118" s="9"/>
@@ -2444,7 +2502,7 @@
       <c r="O118" s="6"/>
       <c r="P118" s="10"/>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A119" s="6"/>
       <c r="B119" s="6"/>
       <c r="D119" s="9"/>
@@ -2458,7 +2516,7 @@
       <c r="O119" s="6"/>
       <c r="P119" s="6"/>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A120" s="6"/>
       <c r="B120" s="6"/>
       <c r="D120" s="9"/>
@@ -2472,7 +2530,7 @@
       <c r="O120" s="6"/>
       <c r="P120" s="6"/>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A121" s="6"/>
       <c r="B121" s="6"/>
       <c r="D121" s="9"/>
@@ -2487,7 +2545,7 @@
       <c r="O121" s="6"/>
       <c r="P121" s="10"/>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A122" s="8"/>
       <c r="B122" s="8"/>
       <c r="D122" s="9"/>
@@ -2501,7 +2559,7 @@
       <c r="O122" s="6"/>
       <c r="P122" s="10"/>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A123" s="6"/>
       <c r="B123" s="6"/>
       <c r="D123" s="9"/>
@@ -2515,7 +2573,7 @@
       <c r="O123" s="6"/>
       <c r="P123" s="6"/>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A124" s="8"/>
       <c r="B124" s="8"/>
       <c r="D124" s="9"/>
@@ -2529,7 +2587,7 @@
       <c r="O124" s="6"/>
       <c r="P124" s="10"/>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A125" s="6"/>
       <c r="B125" s="6"/>
       <c r="D125" s="9"/>
@@ -2543,7 +2601,7 @@
       <c r="O125" s="6"/>
       <c r="P125" s="6"/>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A126" s="6"/>
       <c r="B126" s="6"/>
       <c r="D126" s="9"/>
@@ -2557,7 +2615,7 @@
       <c r="O126" s="6"/>
       <c r="P126" s="6"/>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A127" s="6"/>
       <c r="B127" s="6"/>
       <c r="D127" s="9"/>
@@ -2571,7 +2629,7 @@
       <c r="O127" s="6"/>
       <c r="P127" s="6"/>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A128" s="6"/>
       <c r="B128" s="6"/>
       <c r="D128" s="9"/>
@@ -2585,7 +2643,7 @@
       <c r="O128" s="6"/>
       <c r="P128" s="6"/>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A129" s="6"/>
       <c r="B129" s="6"/>
       <c r="D129" s="9"/>
@@ -2599,7 +2657,7 @@
       <c r="O129" s="6"/>
       <c r="P129" s="6"/>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A130" s="6"/>
       <c r="B130" s="6"/>
       <c r="D130" s="9"/>
@@ -2613,7 +2671,7 @@
       <c r="O130" s="6"/>
       <c r="P130" s="6"/>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A131" s="6"/>
       <c r="B131" s="6"/>
       <c r="D131" s="9"/>
@@ -2627,7 +2685,7 @@
       <c r="O131" s="6"/>
       <c r="P131" s="6"/>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A132" s="6"/>
       <c r="B132" s="6"/>
       <c r="D132" s="9"/>
@@ -2641,7 +2699,7 @@
       <c r="O132" s="6"/>
       <c r="P132" s="6"/>
     </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A133" s="6"/>
       <c r="B133" s="6"/>
       <c r="D133" s="9"/>
@@ -2655,7 +2713,7 @@
       <c r="O133" s="6"/>
       <c r="P133" s="6"/>
     </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A134" s="6"/>
       <c r="B134" s="6"/>
       <c r="D134" s="9"/>
@@ -2669,7 +2727,7 @@
       <c r="O134" s="6"/>
       <c r="P134" s="6"/>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A135" s="6"/>
       <c r="B135" s="6"/>
       <c r="D135" s="9"/>
@@ -2683,7 +2741,7 @@
       <c r="O135" s="6"/>
       <c r="P135" s="6"/>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A136" s="6"/>
       <c r="B136" s="6"/>
       <c r="D136" s="9"/>
@@ -2697,7 +2755,7 @@
       <c r="O136" s="6"/>
       <c r="P136" s="6"/>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A137" s="6"/>
       <c r="B137" s="6"/>
       <c r="D137" s="9"/>
@@ -2711,7 +2769,7 @@
       <c r="O137" s="6"/>
       <c r="P137" s="6"/>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A138" s="6"/>
       <c r="B138" s="6"/>
       <c r="D138" s="9"/>
@@ -2725,7 +2783,7 @@
       <c r="O138" s="6"/>
       <c r="P138" s="6"/>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A139" s="6"/>
       <c r="B139" s="6"/>
       <c r="D139" s="9"/>
@@ -2739,7 +2797,7 @@
       <c r="O139" s="6"/>
       <c r="P139" s="6"/>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A140" s="6"/>
       <c r="B140" s="6"/>
       <c r="D140" s="9"/>
@@ -2753,7 +2811,7 @@
       <c r="O140" s="6"/>
       <c r="P140" s="6"/>
     </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A141" s="6"/>
       <c r="B141" s="6"/>
       <c r="D141" s="9"/>
@@ -2767,7 +2825,7 @@
       <c r="O141" s="6"/>
       <c r="P141" s="6"/>
     </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A142" s="6"/>
       <c r="B142" s="6"/>
       <c r="D142" s="9"/>
@@ -2781,7 +2839,7 @@
       <c r="O142" s="6"/>
       <c r="P142" s="6"/>
     </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A143" s="6"/>
       <c r="B143" s="6"/>
       <c r="D143" s="9"/>
@@ -2795,7 +2853,7 @@
       <c r="O143" s="6"/>
       <c r="P143" s="6"/>
     </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A144" s="6"/>
       <c r="B144" s="6"/>
       <c r="D144" s="9"/>
@@ -2809,7 +2867,7 @@
       <c r="O144" s="6"/>
       <c r="P144" s="6"/>
     </row>
-    <row r="145" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A145" s="6"/>
       <c r="B145" s="6"/>
       <c r="D145" s="9"/>
@@ -2823,7 +2881,7 @@
       <c r="O145" s="6"/>
       <c r="P145" s="6"/>
     </row>
-    <row r="146" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A146" s="6"/>
       <c r="B146" s="6"/>
       <c r="D146" s="9"/>
@@ -2837,7 +2895,7 @@
       <c r="O146" s="6"/>
       <c r="P146" s="6"/>
     </row>
-    <row r="147" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A147" s="6"/>
       <c r="B147" s="6"/>
       <c r="D147" s="9"/>
@@ -2851,7 +2909,7 @@
       <c r="O147" s="6"/>
       <c r="P147" s="6"/>
     </row>
-    <row r="148" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A148" s="6"/>
       <c r="B148" s="6"/>
       <c r="D148" s="9"/>
@@ -2865,7 +2923,7 @@
       <c r="O148" s="6"/>
       <c r="P148" s="6"/>
     </row>
-    <row r="149" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A149" s="6"/>
       <c r="B149" s="6"/>
       <c r="D149" s="9"/>
@@ -2879,7 +2937,7 @@
       <c r="O149" s="6"/>
       <c r="P149" s="6"/>
     </row>
-    <row r="150" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A150" s="6"/>
       <c r="B150" s="6"/>
       <c r="D150" s="9"/>
@@ -2893,7 +2951,7 @@
       <c r="O150" s="6"/>
       <c r="P150" s="6"/>
     </row>
-    <row r="151" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A151" s="6"/>
       <c r="B151" s="6"/>
       <c r="D151" s="9"/>
@@ -2907,7 +2965,7 @@
       <c r="O151" s="6"/>
       <c r="P151" s="6"/>
     </row>
-    <row r="152" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A152" s="6"/>
       <c r="B152" s="6"/>
       <c r="D152" s="9"/>
@@ -2921,7 +2979,7 @@
       <c r="O152" s="6"/>
       <c r="P152" s="6"/>
     </row>
-    <row r="153" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A153" s="6"/>
       <c r="B153" s="6"/>
       <c r="D153" s="9"/>
@@ -2935,7 +2993,7 @@
       <c r="O153" s="6"/>
       <c r="P153" s="6"/>
     </row>
-    <row r="154" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A154" s="6"/>
       <c r="B154" s="6"/>
       <c r="D154" s="9"/>
@@ -2949,7 +3007,7 @@
       <c r="O154" s="6"/>
       <c r="P154" s="6"/>
     </row>
-    <row r="155" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A155" s="6"/>
       <c r="B155" s="6"/>
       <c r="D155" s="9"/>
@@ -2963,7 +3021,7 @@
       <c r="O155" s="6"/>
       <c r="P155" s="6"/>
     </row>
-    <row r="156" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A156" s="6"/>
       <c r="B156" s="6"/>
       <c r="D156" s="9"/>
@@ -2977,7 +3035,7 @@
       <c r="O156" s="6"/>
       <c r="P156" s="6"/>
     </row>
-    <row r="157" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A157" s="6"/>
       <c r="B157" s="6"/>
       <c r="D157" s="9"/>
@@ -2991,7 +3049,7 @@
       <c r="O157" s="6"/>
       <c r="P157" s="6"/>
     </row>
-    <row r="158" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A158" s="6"/>
       <c r="B158" s="6"/>
       <c r="D158" s="9"/>
@@ -3005,7 +3063,7 @@
       <c r="O158" s="6"/>
       <c r="P158" s="6"/>
     </row>
-    <row r="159" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A159" s="6"/>
       <c r="B159" s="6"/>
       <c r="D159" s="9"/>
@@ -3019,7 +3077,7 @@
       <c r="O159" s="6"/>
       <c r="P159" s="6"/>
     </row>
-    <row r="160" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A160" s="6"/>
       <c r="B160" s="6"/>
       <c r="D160" s="9"/>
@@ -3034,7 +3092,7 @@
       <c r="O160" s="6"/>
       <c r="P160" s="6"/>
     </row>
-    <row r="161" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A161" s="6"/>
       <c r="B161" s="6"/>
       <c r="D161" s="9"/>
@@ -3048,7 +3106,7 @@
       <c r="O161" s="6"/>
       <c r="P161" s="6"/>
     </row>
-    <row r="162" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A162" s="6"/>
       <c r="B162" s="6"/>
       <c r="D162" s="9"/>
@@ -3062,7 +3120,7 @@
       <c r="O162" s="6"/>
       <c r="P162" s="6"/>
     </row>
-    <row r="163" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A163" s="6"/>
       <c r="B163" s="6"/>
       <c r="D163" s="9"/>
@@ -3076,7 +3134,7 @@
       <c r="O163" s="6"/>
       <c r="P163" s="6"/>
     </row>
-    <row r="164" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A164" s="6"/>
       <c r="B164" s="6"/>
       <c r="D164" s="9"/>
@@ -3090,7 +3148,7 @@
       <c r="O164" s="6"/>
       <c r="P164" s="6"/>
     </row>
-    <row r="165" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A165" s="6"/>
       <c r="B165" s="6"/>
       <c r="D165" s="9"/>
@@ -3104,7 +3162,7 @@
       <c r="O165" s="6"/>
       <c r="P165" s="6"/>
     </row>
-    <row r="166" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A166" s="6"/>
       <c r="B166" s="6"/>
       <c r="D166" s="9"/>
@@ -3118,7 +3176,7 @@
       <c r="O166" s="6"/>
       <c r="P166" s="6"/>
     </row>
-    <row r="167" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A167" s="6"/>
       <c r="B167" s="6"/>
       <c r="D167" s="9"/>
@@ -3133,7 +3191,7 @@
       <c r="O167" s="6"/>
       <c r="P167" s="6"/>
     </row>
-    <row r="168" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A168" s="8"/>
       <c r="B168" s="8"/>
       <c r="D168" s="9"/>
@@ -3148,7 +3206,7 @@
       <c r="O168" s="6"/>
       <c r="P168" s="6"/>
     </row>
-    <row r="169" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A169" s="8"/>
       <c r="B169" s="8"/>
       <c r="D169" s="9"/>
@@ -3163,7 +3221,7 @@
       <c r="O169" s="6"/>
       <c r="P169" s="6"/>
     </row>
-    <row r="170" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A170" s="8"/>
       <c r="B170" s="8"/>
       <c r="D170" s="9"/>
@@ -3178,7 +3236,7 @@
       <c r="O170" s="6"/>
       <c r="P170" s="6"/>
     </row>
-    <row r="171" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A171" s="6"/>
       <c r="B171" s="6"/>
       <c r="D171" s="9"/>
@@ -3192,7 +3250,7 @@
       <c r="O171" s="6"/>
       <c r="P171" s="6"/>
     </row>
-    <row r="172" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A172" s="8"/>
       <c r="B172" s="8"/>
       <c r="D172" s="9"/>
@@ -3207,7 +3265,7 @@
       <c r="O172" s="6"/>
       <c r="P172" s="6"/>
     </row>
-    <row r="173" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A173" s="8"/>
       <c r="B173" s="8"/>
       <c r="D173" s="9"/>
@@ -3222,7 +3280,7 @@
       <c r="O173" s="6"/>
       <c r="P173" s="6"/>
     </row>
-    <row r="174" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A174" s="6"/>
       <c r="B174" s="6"/>
       <c r="D174" s="9"/>
@@ -3236,7 +3294,7 @@
       <c r="O174" s="6"/>
       <c r="P174" s="6"/>
     </row>
-    <row r="175" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A175" s="8"/>
       <c r="B175" s="8"/>
       <c r="D175" s="9"/>
@@ -3251,7 +3309,7 @@
       <c r="O175" s="6"/>
       <c r="P175" s="6"/>
     </row>
-    <row r="176" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A176" s="6"/>
       <c r="B176" s="6"/>
       <c r="D176" s="9"/>
@@ -3265,7 +3323,7 @@
       <c r="O176" s="6"/>
       <c r="P176" s="6"/>
     </row>
-    <row r="177" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A177" s="6"/>
       <c r="B177" s="6"/>
       <c r="D177" s="9"/>
@@ -3279,7 +3337,7 @@
       <c r="O177" s="6"/>
       <c r="P177" s="6"/>
     </row>
-    <row r="178" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A178" s="8"/>
       <c r="B178" s="8"/>
       <c r="D178" s="9"/>
@@ -3293,7 +3351,7 @@
       <c r="O178" s="6"/>
       <c r="P178" s="6"/>
     </row>
-    <row r="179" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A179" s="8"/>
       <c r="B179" s="8"/>
       <c r="D179" s="9"/>
@@ -3308,7 +3366,7 @@
       <c r="O179" s="6"/>
       <c r="P179" s="6"/>
     </row>
-    <row r="180" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A180" s="6"/>
       <c r="B180" s="6"/>
       <c r="D180" s="9"/>
@@ -3322,7 +3380,7 @@
       <c r="O180" s="6"/>
       <c r="P180" s="6"/>
     </row>
-    <row r="181" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A181" s="6"/>
       <c r="B181" s="6"/>
       <c r="D181" s="9"/>
@@ -3336,7 +3394,7 @@
       <c r="O181" s="6"/>
       <c r="P181" s="6"/>
     </row>
-    <row r="182" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A182" s="8"/>
       <c r="B182" s="8"/>
       <c r="D182" s="9"/>
@@ -3351,7 +3409,7 @@
       <c r="O182" s="6"/>
       <c r="P182" s="6"/>
     </row>
-    <row r="183" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A183" s="8"/>
       <c r="B183" s="8"/>
       <c r="D183" s="9"/>
@@ -3365,7 +3423,7 @@
       <c r="O183" s="6"/>
       <c r="P183" s="6"/>
     </row>
-    <row r="184" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A184" s="8"/>
       <c r="B184" s="8"/>
       <c r="D184" s="9"/>
@@ -3380,7 +3438,7 @@
       <c r="O184" s="6"/>
       <c r="P184" s="6"/>
     </row>
-    <row r="185" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A185" s="6"/>
       <c r="B185" s="6"/>
       <c r="D185" s="9"/>
@@ -3394,7 +3452,7 @@
       <c r="O185" s="6"/>
       <c r="P185" s="6"/>
     </row>
-    <row r="186" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A186" s="8"/>
       <c r="B186" s="8"/>
       <c r="D186" s="9"/>
@@ -3409,7 +3467,7 @@
       <c r="O186" s="6"/>
       <c r="P186" s="6"/>
     </row>
-    <row r="187" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A187" s="8"/>
       <c r="B187" s="8"/>
       <c r="D187" s="9"/>
@@ -3423,7 +3481,7 @@
       <c r="O187" s="6"/>
       <c r="P187" s="6"/>
     </row>
-    <row r="188" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A188" s="8"/>
       <c r="B188" s="8"/>
       <c r="D188" s="9"/>
@@ -3437,7 +3495,7 @@
       <c r="O188" s="6"/>
       <c r="P188" s="6"/>
     </row>
-    <row r="189" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A189" s="8"/>
       <c r="B189" s="8"/>
       <c r="D189" s="9"/>
@@ -3452,7 +3510,7 @@
       <c r="O189" s="6"/>
       <c r="P189" s="6"/>
     </row>
-    <row r="190" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A190" s="6"/>
       <c r="B190" s="6"/>
       <c r="D190" s="9"/>
@@ -3466,7 +3524,7 @@
       <c r="O190" s="6"/>
       <c r="P190" s="6"/>
     </row>
-    <row r="191" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A191" s="6"/>
       <c r="B191" s="6"/>
       <c r="D191" s="9"/>
@@ -3480,7 +3538,7 @@
       <c r="O191" s="6"/>
       <c r="P191" s="6"/>
     </row>
-    <row r="192" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A192" s="6"/>
       <c r="B192" s="6"/>
       <c r="D192" s="9"/>
@@ -3494,7 +3552,7 @@
       <c r="O192" s="6"/>
       <c r="P192" s="6"/>
     </row>
-    <row r="193" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A193" s="8"/>
       <c r="B193" s="8"/>
       <c r="D193" s="9"/>
@@ -3508,7 +3566,7 @@
       <c r="O193" s="6"/>
       <c r="P193" s="6"/>
     </row>
-    <row r="194" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A194" s="8"/>
       <c r="B194" s="8"/>
       <c r="D194" s="9"/>
@@ -3522,7 +3580,7 @@
       <c r="O194" s="6"/>
       <c r="P194" s="6"/>
     </row>
-    <row r="195" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A195" s="8"/>
       <c r="B195" s="8"/>
       <c r="D195" s="9"/>
@@ -3536,7 +3594,7 @@
       <c r="O195" s="6"/>
       <c r="P195" s="6"/>
     </row>
-    <row r="196" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A196" s="6"/>
       <c r="B196" s="6"/>
       <c r="D196" s="9"/>
@@ -3551,7 +3609,7 @@
       <c r="O196" s="6"/>
       <c r="P196" s="6"/>
     </row>
-    <row r="197" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A197" s="8"/>
       <c r="B197" s="8"/>
       <c r="D197" s="9"/>
@@ -3565,7 +3623,7 @@
       <c r="O197" s="6"/>
       <c r="P197" s="6"/>
     </row>
-    <row r="198" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A198" s="6"/>
       <c r="B198" s="6"/>
       <c r="D198" s="9"/>
@@ -3579,7 +3637,7 @@
       <c r="O198" s="6"/>
       <c r="P198" s="6"/>
     </row>
-    <row r="199" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A199" s="6"/>
       <c r="B199" s="6"/>
       <c r="D199" s="9"/>
@@ -3593,7 +3651,7 @@
       <c r="O199" s="6"/>
       <c r="P199" s="6"/>
     </row>
-    <row r="200" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A200" s="6"/>
       <c r="B200" s="6"/>
       <c r="D200" s="9"/>
@@ -3607,7 +3665,7 @@
       <c r="O200" s="6"/>
       <c r="P200" s="6"/>
     </row>
-    <row r="201" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A201" s="6"/>
       <c r="B201" s="6"/>
       <c r="D201" s="9"/>
@@ -3621,7 +3679,7 @@
       <c r="O201" s="6"/>
       <c r="P201" s="6"/>
     </row>
-    <row r="202" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A202" s="6"/>
       <c r="B202" s="6"/>
       <c r="D202" s="9"/>
@@ -3635,7 +3693,7 @@
       <c r="O202" s="6"/>
       <c r="P202" s="6"/>
     </row>
-    <row r="203" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A203" s="6"/>
       <c r="B203" s="6"/>
       <c r="D203" s="9"/>
@@ -3649,7 +3707,7 @@
       <c r="O203" s="6"/>
       <c r="P203" s="6"/>
     </row>
-    <row r="204" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A204" s="6"/>
       <c r="B204" s="6"/>
       <c r="D204" s="9"/>
@@ -3663,7 +3721,7 @@
       <c r="O204" s="6"/>
       <c r="P204" s="6"/>
     </row>
-    <row r="205" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A205" s="6"/>
       <c r="B205" s="6"/>
       <c r="D205" s="9"/>
@@ -3677,7 +3735,7 @@
       <c r="O205" s="6"/>
       <c r="P205" s="6"/>
     </row>
-    <row r="206" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A206" s="6"/>
       <c r="B206" s="6"/>
       <c r="D206" s="9"/>
@@ -3691,7 +3749,7 @@
       <c r="O206" s="6"/>
       <c r="P206" s="6"/>
     </row>
-    <row r="207" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A207" s="6"/>
       <c r="B207" s="6"/>
       <c r="D207" s="9"/>
@@ -3705,7 +3763,7 @@
       <c r="O207" s="6"/>
       <c r="P207" s="6"/>
     </row>
-    <row r="208" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A208" s="6"/>
       <c r="B208" s="6"/>
       <c r="D208" s="9"/>
@@ -3719,7 +3777,7 @@
       <c r="O208" s="6"/>
       <c r="P208" s="6"/>
     </row>
-    <row r="209" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A209" s="6"/>
       <c r="B209" s="6"/>
       <c r="D209" s="9"/>
@@ -3733,7 +3791,7 @@
       <c r="O209" s="6"/>
       <c r="P209" s="6"/>
     </row>
-    <row r="210" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A210" s="6"/>
       <c r="B210" s="6"/>
       <c r="D210" s="9"/>
@@ -3747,7 +3805,7 @@
       <c r="O210" s="6"/>
       <c r="P210" s="6"/>
     </row>
-    <row r="211" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A211" s="6"/>
       <c r="B211" s="6"/>
       <c r="D211" s="9"/>
@@ -3761,7 +3819,7 @@
       <c r="O211" s="6"/>
       <c r="P211" s="6"/>
     </row>
-    <row r="212" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A212" s="6"/>
       <c r="B212" s="6"/>
       <c r="D212" s="9"/>
@@ -3775,7 +3833,7 @@
       <c r="O212" s="6"/>
       <c r="P212" s="6"/>
     </row>
-    <row r="213" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A213" s="6"/>
       <c r="B213" s="6"/>
       <c r="D213" s="9"/>
@@ -3789,7 +3847,7 @@
       <c r="O213" s="6"/>
       <c r="P213" s="6"/>
     </row>
-    <row r="214" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A214" s="6"/>
       <c r="B214" s="6"/>
       <c r="D214" s="9"/>
@@ -3803,7 +3861,7 @@
       <c r="O214" s="6"/>
       <c r="P214" s="6"/>
     </row>
-    <row r="215" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A215" s="6"/>
       <c r="B215" s="6"/>
       <c r="D215" s="9"/>
@@ -3817,7 +3875,7 @@
       <c r="O215" s="6"/>
       <c r="P215" s="6"/>
     </row>
-    <row r="216" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A216" s="6"/>
       <c r="B216" s="6"/>
       <c r="D216" s="9"/>
@@ -3832,7 +3890,7 @@
       <c r="O216" s="6"/>
       <c r="P216" s="6"/>
     </row>
-    <row r="217" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A217" s="6"/>
       <c r="B217" s="6"/>
       <c r="D217" s="9"/>
@@ -3846,7 +3904,7 @@
       <c r="O217" s="6"/>
       <c r="P217" s="6"/>
     </row>
-    <row r="218" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A218" s="6"/>
       <c r="B218" s="6"/>
       <c r="D218" s="9"/>
@@ -3861,7 +3919,7 @@
       <c r="O218" s="6"/>
       <c r="P218" s="6"/>
     </row>
-    <row r="219" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A219" s="6"/>
       <c r="B219" s="6"/>
       <c r="D219" s="9"/>
@@ -3875,7 +3933,7 @@
       <c r="O219" s="6"/>
       <c r="P219" s="6"/>
     </row>
-    <row r="220" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A220" s="6"/>
       <c r="B220" s="6"/>
       <c r="D220" s="9"/>
@@ -3889,7 +3947,7 @@
       <c r="O220" s="6"/>
       <c r="P220" s="6"/>
     </row>
-    <row r="221" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A221" s="6"/>
       <c r="B221" s="6"/>
       <c r="D221" s="9"/>
@@ -3903,7 +3961,7 @@
       <c r="O221" s="6"/>
       <c r="P221" s="8"/>
     </row>
-    <row r="222" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A222" s="6"/>
       <c r="B222" s="6"/>
       <c r="D222" s="9"/>
@@ -3917,7 +3975,7 @@
       <c r="O222" s="6"/>
       <c r="P222" s="6"/>
     </row>
-    <row r="223" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A223" s="6"/>
       <c r="B223" s="6"/>
       <c r="D223" s="9"/>
@@ -3931,7 +3989,7 @@
       <c r="O223" s="6"/>
       <c r="P223" s="6"/>
     </row>
-    <row r="224" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A224" s="6"/>
       <c r="B224" s="6"/>
       <c r="D224" s="9"/>
@@ -3945,7 +4003,7 @@
       <c r="O224" s="6"/>
       <c r="P224" s="6"/>
     </row>
-    <row r="225" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A225" s="6"/>
       <c r="B225" s="6"/>
       <c r="D225" s="9"/>
@@ -3959,7 +4017,7 @@
       <c r="O225" s="6"/>
       <c r="P225" s="6"/>
     </row>
-    <row r="226" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A226" s="6"/>
       <c r="B226" s="6"/>
       <c r="D226" s="9"/>
@@ -3973,7 +4031,7 @@
       <c r="O226" s="6"/>
       <c r="P226" s="6"/>
     </row>
-    <row r="227" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A227" s="6"/>
       <c r="B227" s="6"/>
       <c r="D227" s="9"/>
@@ -3987,7 +4045,7 @@
       <c r="O227" s="6"/>
       <c r="P227" s="6"/>
     </row>
-    <row r="228" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A228" s="6"/>
       <c r="B228" s="6"/>
       <c r="D228" s="9"/>
@@ -4001,7 +4059,7 @@
       <c r="O228" s="6"/>
       <c r="P228" s="6"/>
     </row>
-    <row r="229" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A229" s="6"/>
       <c r="B229" s="6"/>
       <c r="D229" s="9"/>
@@ -4015,7 +4073,7 @@
       <c r="O229" s="6"/>
       <c r="P229" s="6"/>
     </row>
-    <row r="230" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A230" s="6"/>
       <c r="B230" s="6"/>
       <c r="D230" s="9"/>
@@ -4029,7 +4087,7 @@
       <c r="O230" s="6"/>
       <c r="P230" s="6"/>
     </row>
-    <row r="231" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A231" s="6"/>
       <c r="B231" s="6"/>
       <c r="D231" s="9"/>
@@ -4043,7 +4101,7 @@
       <c r="O231" s="6"/>
       <c r="P231" s="6"/>
     </row>
-    <row r="232" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A232" s="6"/>
       <c r="B232" s="6"/>
       <c r="D232" s="9"/>
@@ -4057,7 +4115,7 @@
       <c r="O232" s="6"/>
       <c r="P232" s="6"/>
     </row>
-    <row r="233" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A233" s="6"/>
       <c r="B233" s="6"/>
       <c r="D233" s="9"/>
@@ -4071,7 +4129,7 @@
       <c r="O233" s="6"/>
       <c r="P233" s="6"/>
     </row>
-    <row r="234" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A234" s="6"/>
       <c r="B234" s="6"/>
       <c r="D234" s="9"/>
@@ -4085,7 +4143,7 @@
       <c r="O234" s="6"/>
       <c r="P234" s="6"/>
     </row>
-    <row r="235" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A235" s="6"/>
       <c r="B235" s="6"/>
       <c r="D235" s="9"/>
@@ -4099,7 +4157,7 @@
       <c r="O235" s="6"/>
       <c r="P235" s="6"/>
     </row>
-    <row r="236" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A236" s="6"/>
       <c r="B236" s="6"/>
       <c r="D236" s="9"/>
@@ -4113,7 +4171,7 @@
       <c r="O236" s="6"/>
       <c r="P236" s="6"/>
     </row>
-    <row r="237" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A237" s="6"/>
       <c r="B237" s="6"/>
       <c r="D237" s="9"/>
@@ -4127,7 +4185,7 @@
       <c r="O237" s="6"/>
       <c r="P237" s="6"/>
     </row>
-    <row r="238" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A238" s="6"/>
       <c r="B238" s="6"/>
       <c r="D238" s="9"/>
@@ -4141,7 +4199,7 @@
       <c r="O238" s="6"/>
       <c r="P238" s="6"/>
     </row>
-    <row r="239" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A239" s="6"/>
       <c r="B239" s="6"/>
       <c r="D239" s="9"/>
@@ -4156,7 +4214,7 @@
       <c r="O239" s="6"/>
       <c r="P239" s="6"/>
     </row>
-    <row r="240" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A240" s="6"/>
       <c r="B240" s="6"/>
       <c r="D240" s="9"/>
@@ -4170,7 +4228,7 @@
       <c r="O240" s="6"/>
       <c r="P240" s="6"/>
     </row>
-    <row r="241" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A241" s="6"/>
       <c r="B241" s="6"/>
       <c r="D241" s="9"/>
@@ -4184,7 +4242,7 @@
       <c r="O241" s="6"/>
       <c r="P241" s="6"/>
     </row>
-    <row r="242" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A242" s="6"/>
       <c r="B242" s="6"/>
       <c r="D242" s="9"/>
@@ -4199,7 +4257,7 @@
       <c r="O242" s="6"/>
       <c r="P242" s="6"/>
     </row>
-    <row r="243" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A243" s="6"/>
       <c r="B243" s="6"/>
       <c r="D243" s="9"/>
@@ -4213,7 +4271,7 @@
       <c r="O243" s="6"/>
       <c r="P243" s="6"/>
     </row>
-    <row r="244" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A244" s="6"/>
       <c r="B244" s="6"/>
       <c r="D244" s="9"/>
@@ -4227,7 +4285,7 @@
       <c r="O244" s="6"/>
       <c r="P244" s="6"/>
     </row>
-    <row r="245" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A245" s="6"/>
       <c r="B245" s="6"/>
       <c r="D245" s="9"/>
@@ -4241,7 +4299,7 @@
       <c r="O245" s="6"/>
       <c r="P245" s="6"/>
     </row>
-    <row r="246" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A246" s="6"/>
       <c r="B246" s="6"/>
       <c r="D246" s="9"/>
@@ -4255,7 +4313,7 @@
       <c r="O246" s="6"/>
       <c r="P246" s="6"/>
     </row>
-    <row r="247" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A247" s="6"/>
       <c r="B247" s="6"/>
       <c r="D247" s="9"/>
@@ -4269,7 +4327,7 @@
       <c r="O247" s="6"/>
       <c r="P247" s="6"/>
     </row>
-    <row r="248" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A248" s="6"/>
       <c r="B248" s="6"/>
       <c r="D248" s="9"/>
@@ -4283,7 +4341,7 @@
       <c r="O248" s="6"/>
       <c r="P248" s="6"/>
     </row>
-    <row r="249" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A249" s="6"/>
       <c r="B249" s="6"/>
       <c r="D249" s="9"/>
@@ -4297,7 +4355,7 @@
       <c r="O249" s="6"/>
       <c r="P249" s="6"/>
     </row>
-    <row r="250" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A250" s="6"/>
       <c r="B250" s="6"/>
       <c r="D250" s="9"/>
@@ -4311,7 +4369,7 @@
       <c r="O250" s="6"/>
       <c r="P250" s="6"/>
     </row>
-    <row r="251" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A251" s="6"/>
       <c r="B251" s="6"/>
       <c r="D251" s="9"/>
@@ -4325,7 +4383,7 @@
       <c r="O251" s="6"/>
       <c r="P251" s="6"/>
     </row>
-    <row r="252" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A252" s="6"/>
       <c r="B252" s="6"/>
       <c r="D252" s="9"/>
@@ -4339,7 +4397,7 @@
       <c r="O252" s="6"/>
       <c r="P252" s="6"/>
     </row>
-    <row r="253" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A253" s="6"/>
       <c r="B253" s="6"/>
       <c r="D253" s="9"/>
@@ -4353,7 +4411,7 @@
       <c r="O253" s="6"/>
       <c r="P253" s="6"/>
     </row>
-    <row r="254" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A254" s="6"/>
       <c r="B254" s="6"/>
       <c r="D254" s="9"/>
@@ -4367,7 +4425,7 @@
       <c r="O254" s="6"/>
       <c r="P254" s="6"/>
     </row>
-    <row r="255" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A255" s="6"/>
       <c r="B255" s="6"/>
       <c r="D255" s="9"/>
@@ -4381,7 +4439,7 @@
       <c r="O255" s="6"/>
       <c r="P255" s="6"/>
     </row>
-    <row r="256" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A256" s="6"/>
       <c r="B256" s="6"/>
       <c r="D256" s="9"/>
@@ -4395,7 +4453,7 @@
       <c r="O256" s="6"/>
       <c r="P256" s="6"/>
     </row>
-    <row r="257" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A257" s="6"/>
       <c r="B257" s="6"/>
       <c r="D257" s="9"/>
@@ -4409,7 +4467,7 @@
       <c r="O257" s="6"/>
       <c r="P257" s="6"/>
     </row>
-    <row r="258" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A258" s="6"/>
       <c r="B258" s="6"/>
       <c r="D258" s="9"/>
@@ -4423,7 +4481,7 @@
       <c r="O258" s="6"/>
       <c r="P258" s="6"/>
     </row>
-    <row r="259" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A259" s="6"/>
       <c r="B259" s="6"/>
       <c r="D259" s="9"/>
@@ -4437,7 +4495,7 @@
       <c r="O259" s="6"/>
       <c r="P259" s="6"/>
     </row>
-    <row r="260" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A260" s="6"/>
       <c r="B260" s="6"/>
       <c r="D260" s="9"/>
@@ -4451,7 +4509,7 @@
       <c r="O260" s="6"/>
       <c r="P260" s="6"/>
     </row>
-    <row r="261" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A261" s="6"/>
       <c r="B261" s="6"/>
       <c r="D261" s="9"/>
@@ -4465,7 +4523,7 @@
       <c r="O261" s="6"/>
       <c r="P261" s="6"/>
     </row>
-    <row r="262" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A262" s="6"/>
       <c r="B262" s="6"/>
       <c r="D262" s="9"/>
@@ -4479,7 +4537,7 @@
       <c r="O262" s="6"/>
       <c r="P262" s="6"/>
     </row>
-    <row r="263" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A263" s="6"/>
       <c r="B263" s="6"/>
       <c r="D263" s="9"/>
@@ -4494,7 +4552,7 @@
       <c r="O263" s="6"/>
       <c r="P263" s="6"/>
     </row>
-    <row r="264" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A264" s="6"/>
       <c r="B264" s="6"/>
       <c r="D264" s="9"/>
@@ -4508,7 +4566,7 @@
       <c r="O264" s="6"/>
       <c r="P264" s="6"/>
     </row>
-    <row r="265" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A265" s="6"/>
       <c r="B265" s="6"/>
       <c r="D265" s="9"/>
@@ -4522,7 +4580,7 @@
       <c r="O265" s="6"/>
       <c r="P265" s="6"/>
     </row>
-    <row r="266" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A266" s="6"/>
       <c r="B266" s="6"/>
       <c r="D266" s="9"/>
@@ -4536,7 +4594,7 @@
       <c r="O266" s="6"/>
       <c r="P266" s="6"/>
     </row>
-    <row r="267" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A267" s="6"/>
       <c r="B267" s="6"/>
       <c r="D267" s="9"/>
@@ -4550,7 +4608,7 @@
       <c r="O267" s="6"/>
       <c r="P267" s="6"/>
     </row>
-    <row r="268" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A268" s="6"/>
       <c r="B268" s="6"/>
       <c r="D268" s="9"/>
@@ -4564,7 +4622,7 @@
       <c r="O268" s="6"/>
       <c r="P268" s="6"/>
     </row>
-    <row r="269" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A269" s="6"/>
       <c r="B269" s="6"/>
       <c r="D269" s="9"/>
@@ -4578,7 +4636,7 @@
       <c r="O269" s="8"/>
       <c r="P269" s="6"/>
     </row>
-    <row r="270" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A270" s="6"/>
       <c r="B270" s="6"/>
       <c r="D270" s="9"/>
@@ -4592,7 +4650,7 @@
       <c r="O270" s="6"/>
       <c r="P270" s="6"/>
     </row>
-    <row r="271" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A271" s="6"/>
       <c r="B271" s="6"/>
       <c r="D271" s="9"/>
@@ -4606,7 +4664,7 @@
       <c r="O271" s="6"/>
       <c r="P271" s="6"/>
     </row>
-    <row r="272" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A272" s="6"/>
       <c r="B272" s="6"/>
       <c r="D272" s="9"/>
@@ -4620,7 +4678,7 @@
       <c r="O272" s="6"/>
       <c r="P272" s="6"/>
     </row>
-    <row r="273" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A273" s="8"/>
       <c r="B273" s="8"/>
       <c r="D273" s="9"/>
@@ -4635,7 +4693,7 @@
       <c r="O273" s="6"/>
       <c r="P273" s="6"/>
     </row>
-    <row r="274" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A274" s="6"/>
       <c r="B274" s="6"/>
       <c r="D274" s="9"/>
@@ -4649,7 +4707,7 @@
       <c r="O274" s="6"/>
       <c r="P274" s="6"/>
     </row>
-    <row r="275" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A275" s="6"/>
       <c r="B275" s="6"/>
       <c r="D275" s="9"/>
@@ -4663,7 +4721,7 @@
       <c r="O275" s="6"/>
       <c r="P275" s="6"/>
     </row>
-    <row r="276" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A276" s="6"/>
       <c r="B276" s="6"/>
       <c r="D276" s="9"/>
@@ -4677,7 +4735,7 @@
       <c r="O276" s="6"/>
       <c r="P276" s="6"/>
     </row>
-    <row r="277" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A277" s="6"/>
       <c r="B277" s="6"/>
       <c r="D277" s="9"/>
@@ -4691,7 +4749,7 @@
       <c r="O277" s="6"/>
       <c r="P277" s="6"/>
     </row>
-    <row r="278" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A278" s="6"/>
       <c r="B278" s="6"/>
       <c r="D278" s="9"/>
@@ -4705,7 +4763,7 @@
       <c r="O278" s="6"/>
       <c r="P278" s="6"/>
     </row>
-    <row r="279" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A279" s="6"/>
       <c r="B279" s="6"/>
       <c r="D279" s="9"/>
@@ -4719,7 +4777,7 @@
       <c r="O279" s="6"/>
       <c r="P279" s="6"/>
     </row>
-    <row r="280" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A280" s="6"/>
       <c r="B280" s="6"/>
       <c r="D280" s="9"/>
@@ -4733,7 +4791,7 @@
       <c r="O280" s="6"/>
       <c r="P280" s="6"/>
     </row>
-    <row r="281" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A281" s="6"/>
       <c r="B281" s="6"/>
       <c r="D281" s="9"/>
@@ -4747,7 +4805,7 @@
       <c r="O281" s="6"/>
       <c r="P281" s="6"/>
     </row>
-    <row r="282" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A282" s="6"/>
       <c r="B282" s="6"/>
       <c r="D282" s="9"/>
@@ -4761,7 +4819,7 @@
       <c r="O282" s="6"/>
       <c r="P282" s="6"/>
     </row>
-    <row r="283" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A283" s="6"/>
       <c r="B283" s="6"/>
       <c r="D283" s="9"/>
@@ -4775,7 +4833,7 @@
       <c r="O283" s="6"/>
       <c r="P283" s="6"/>
     </row>
-    <row r="284" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A284" s="6"/>
       <c r="B284" s="6"/>
       <c r="D284" s="9"/>
@@ -4789,7 +4847,7 @@
       <c r="O284" s="6"/>
       <c r="P284" s="6"/>
     </row>
-    <row r="285" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A285" s="6"/>
       <c r="B285" s="6"/>
       <c r="D285" s="9"/>
@@ -4803,7 +4861,7 @@
       <c r="O285" s="6"/>
       <c r="P285" s="6"/>
     </row>
-    <row r="286" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A286" s="6"/>
       <c r="B286" s="6"/>
       <c r="D286" s="9"/>
@@ -4817,7 +4875,7 @@
       <c r="O286" s="6"/>
       <c r="P286" s="6"/>
     </row>
-    <row r="287" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A287" s="6"/>
       <c r="B287" s="6"/>
       <c r="D287" s="9"/>
@@ -4831,7 +4889,7 @@
       <c r="O287" s="6"/>
       <c r="P287" s="6"/>
     </row>
-    <row r="288" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A288" s="6"/>
       <c r="B288" s="6"/>
       <c r="D288" s="9"/>
@@ -4845,7 +4903,7 @@
       <c r="O288" s="6"/>
       <c r="P288" s="6"/>
     </row>
-    <row r="289" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A289" s="6"/>
       <c r="B289" s="6"/>
       <c r="D289" s="9"/>
@@ -4859,7 +4917,7 @@
       <c r="O289" s="6"/>
       <c r="P289" s="6"/>
     </row>
-    <row r="290" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A290" s="6"/>
       <c r="B290" s="6"/>
       <c r="D290" s="9"/>
@@ -4873,7 +4931,7 @@
       <c r="O290" s="6"/>
       <c r="P290" s="6"/>
     </row>
-    <row r="291" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A291" s="6"/>
       <c r="B291" s="6"/>
       <c r="D291" s="9"/>
@@ -4887,7 +4945,7 @@
       <c r="O291" s="6"/>
       <c r="P291" s="6"/>
     </row>
-    <row r="292" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A292" s="6"/>
       <c r="B292" s="6"/>
       <c r="D292" s="9"/>
@@ -4901,7 +4959,7 @@
       <c r="O292" s="6"/>
       <c r="P292" s="6"/>
     </row>
-    <row r="293" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A293" s="6"/>
       <c r="B293" s="6"/>
       <c r="D293" s="9"/>
@@ -4915,7 +4973,7 @@
       <c r="O293" s="6"/>
       <c r="P293" s="6"/>
     </row>
-    <row r="294" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A294" s="6"/>
       <c r="B294" s="6"/>
       <c r="D294" s="9"/>
@@ -4929,7 +4987,7 @@
       <c r="O294" s="6"/>
       <c r="P294" s="6"/>
     </row>
-    <row r="295" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A295" s="6"/>
       <c r="B295" s="6"/>
       <c r="D295" s="9"/>
@@ -4943,7 +5001,7 @@
       <c r="O295" s="6"/>
       <c r="P295" s="6"/>
     </row>
-    <row r="296" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A296" s="6"/>
       <c r="B296" s="6"/>
       <c r="D296" s="9"/>
@@ -4957,7 +5015,7 @@
       <c r="O296" s="6"/>
       <c r="P296" s="6"/>
     </row>
-    <row r="297" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A297" s="6"/>
       <c r="B297" s="6"/>
       <c r="D297" s="9"/>
@@ -4971,7 +5029,7 @@
       <c r="O297" s="6"/>
       <c r="P297" s="6"/>
     </row>
-    <row r="298" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A298" s="6"/>
       <c r="B298" s="6"/>
       <c r="D298" s="9"/>
@@ -4985,7 +5043,7 @@
       <c r="O298" s="6"/>
       <c r="P298" s="6"/>
     </row>
-    <row r="299" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A299" s="6"/>
       <c r="B299" s="6"/>
       <c r="D299" s="9"/>
@@ -4999,7 +5057,7 @@
       <c r="O299" s="6"/>
       <c r="P299" s="6"/>
     </row>
-    <row r="300" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A300" s="6"/>
       <c r="B300" s="6"/>
       <c r="D300" s="9"/>
@@ -5013,7 +5071,7 @@
       <c r="O300" s="6"/>
       <c r="P300" s="6"/>
     </row>
-    <row r="301" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A301" s="6"/>
       <c r="B301" s="6"/>
       <c r="D301" s="9"/>
@@ -5027,7 +5085,7 @@
       <c r="O301" s="6"/>
       <c r="P301" s="6"/>
     </row>
-    <row r="302" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A302" s="6"/>
       <c r="B302" s="6"/>
       <c r="D302" s="9"/>
@@ -5041,7 +5099,7 @@
       <c r="O302" s="6"/>
       <c r="P302" s="6"/>
     </row>
-    <row r="303" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A303" s="6"/>
       <c r="B303" s="6"/>
       <c r="D303" s="9"/>
@@ -5055,7 +5113,7 @@
       <c r="O303" s="6"/>
       <c r="P303" s="6"/>
     </row>
-    <row r="304" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A304" s="6"/>
       <c r="B304" s="6"/>
       <c r="D304" s="9"/>
@@ -5069,7 +5127,7 @@
       <c r="O304" s="6"/>
       <c r="P304" s="6"/>
     </row>
-    <row r="305" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A305" s="6"/>
       <c r="B305" s="6"/>
       <c r="D305" s="9"/>
@@ -5083,7 +5141,7 @@
       <c r="O305" s="6"/>
       <c r="P305" s="6"/>
     </row>
-    <row r="306" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A306" s="8"/>
       <c r="B306" s="8"/>
       <c r="D306" s="18"/>
@@ -5098,7 +5156,7 @@
       <c r="O306" s="6"/>
       <c r="P306" s="8"/>
     </row>
-    <row r="307" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A307" s="6"/>
       <c r="B307" s="6"/>
       <c r="D307" s="9"/>
@@ -5112,7 +5170,7 @@
       <c r="O307" s="6"/>
       <c r="P307" s="6"/>
     </row>
-    <row r="308" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A308" s="6"/>
       <c r="B308" s="6"/>
       <c r="D308" s="9"/>
@@ -5126,7 +5184,7 @@
       <c r="O308" s="6"/>
       <c r="P308" s="6"/>
     </row>
-    <row r="309" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A309" s="6"/>
       <c r="B309" s="6"/>
       <c r="D309" s="9"/>
@@ -5140,7 +5198,7 @@
       <c r="O309" s="6"/>
       <c r="P309" s="15"/>
     </row>
-    <row r="310" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A310" s="8"/>
       <c r="B310" s="8"/>
       <c r="D310" s="18"/>
@@ -5154,7 +5212,7 @@
       <c r="O310" s="6"/>
       <c r="P310" s="8"/>
     </row>
-    <row r="311" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A311" s="6"/>
       <c r="B311" s="6"/>
       <c r="D311" s="9"/>
@@ -5168,7 +5226,7 @@
       <c r="O311" s="6"/>
       <c r="P311" s="6"/>
     </row>
-    <row r="312" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A312" s="8"/>
       <c r="B312" s="8"/>
       <c r="D312" s="18"/>
@@ -5183,7 +5241,7 @@
       <c r="O312" s="6"/>
       <c r="P312" s="8"/>
     </row>
-    <row r="313" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A313" s="6"/>
       <c r="B313" s="6"/>
       <c r="D313" s="9"/>
@@ -5197,7 +5255,7 @@
       <c r="O313" s="6"/>
       <c r="P313" s="6"/>
     </row>
-    <row r="314" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A314" s="6"/>
       <c r="B314" s="6"/>
       <c r="D314" s="9"/>
@@ -5211,7 +5269,7 @@
       <c r="O314" s="6"/>
       <c r="P314" s="6"/>
     </row>
-    <row r="315" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A315" s="6"/>
       <c r="B315" s="6"/>
       <c r="D315" s="9"/>
@@ -5225,7 +5283,7 @@
       <c r="O315" s="6"/>
       <c r="P315" s="6"/>
     </row>
-    <row r="316" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A316" s="8"/>
       <c r="B316" s="8"/>
       <c r="D316" s="18"/>
@@ -5239,7 +5297,7 @@
       <c r="O316" s="6"/>
       <c r="P316" s="8"/>
     </row>
-    <row r="317" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A317" s="8"/>
       <c r="B317" s="8"/>
       <c r="D317" s="18"/>
@@ -5253,7 +5311,7 @@
       <c r="O317" s="6"/>
       <c r="P317" s="8"/>
     </row>
-    <row r="318" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A318" s="6"/>
       <c r="B318" s="6"/>
       <c r="D318" s="9"/>
@@ -5267,7 +5325,7 @@
       <c r="O318" s="6"/>
       <c r="P318" s="6"/>
     </row>
-    <row r="319" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A319" s="6"/>
       <c r="B319" s="6"/>
       <c r="D319" s="9"/>
@@ -5281,7 +5339,7 @@
       <c r="O319" s="6"/>
       <c r="P319" s="6"/>
     </row>
-    <row r="320" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A320" s="6"/>
       <c r="B320" s="6"/>
       <c r="D320" s="9"/>
@@ -5295,7 +5353,7 @@
       <c r="O320" s="6"/>
       <c r="P320" s="6"/>
     </row>
-    <row r="321" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A321" s="6"/>
       <c r="B321" s="6"/>
       <c r="D321" s="9"/>
@@ -5309,7 +5367,7 @@
       <c r="O321" s="6"/>
       <c r="P321" s="6"/>
     </row>
-    <row r="322" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A322" s="6"/>
       <c r="B322" s="6"/>
       <c r="D322" s="9"/>
@@ -5323,7 +5381,7 @@
       <c r="O322" s="6"/>
       <c r="P322" s="6"/>
     </row>
-    <row r="323" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A323" s="6"/>
       <c r="B323" s="6"/>
       <c r="D323" s="9"/>
@@ -5337,7 +5395,7 @@
       <c r="O323" s="6"/>
       <c r="P323" s="6"/>
     </row>
-    <row r="324" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A324" s="6"/>
       <c r="B324" s="6"/>
       <c r="D324" s="9"/>
@@ -5352,7 +5410,7 @@
       <c r="O324" s="6"/>
       <c r="P324" s="6"/>
     </row>
-    <row r="325" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A325" s="6"/>
       <c r="B325" s="6"/>
       <c r="D325" s="9"/>
@@ -5366,7 +5424,7 @@
       <c r="O325" s="6"/>
       <c r="P325" s="6"/>
     </row>
-    <row r="326" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A326" s="6"/>
       <c r="B326" s="6"/>
       <c r="D326" s="9"/>
@@ -5380,7 +5438,7 @@
       <c r="O326" s="6"/>
       <c r="P326" s="6"/>
     </row>
-    <row r="327" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A327" s="6"/>
       <c r="B327" s="6"/>
       <c r="D327" s="9"/>
@@ -5394,7 +5452,7 @@
       <c r="O327" s="6"/>
       <c r="P327" s="6"/>
     </row>
-    <row r="328" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A328" s="6"/>
       <c r="B328" s="6"/>
       <c r="D328" s="9"/>
@@ -5408,7 +5466,7 @@
       <c r="O328" s="6"/>
       <c r="P328" s="6"/>
     </row>
-    <row r="329" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A329" s="6"/>
       <c r="B329" s="6"/>
       <c r="D329" s="9"/>
@@ -5422,7 +5480,7 @@
       <c r="O329" s="6"/>
       <c r="P329" s="6"/>
     </row>
-    <row r="330" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A330" s="6"/>
       <c r="B330" s="6"/>
       <c r="D330" s="9"/>
@@ -5436,7 +5494,7 @@
       <c r="O330" s="6"/>
       <c r="P330" s="6"/>
     </row>
-    <row r="331" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A331" s="6"/>
       <c r="B331" s="6"/>
       <c r="D331" s="9"/>
@@ -5450,7 +5508,7 @@
       <c r="O331" s="6"/>
       <c r="P331" s="6"/>
     </row>
-    <row r="332" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A332" s="6"/>
       <c r="B332" s="6"/>
       <c r="D332" s="9"/>
@@ -5464,7 +5522,7 @@
       <c r="O332" s="6"/>
       <c r="P332" s="6"/>
     </row>
-    <row r="333" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A333" s="6"/>
       <c r="B333" s="6"/>
       <c r="D333" s="9"/>
@@ -5478,7 +5536,7 @@
       <c r="O333" s="6"/>
       <c r="P333" s="6"/>
     </row>
-    <row r="334" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A334" s="6"/>
       <c r="B334" s="6"/>
       <c r="D334" s="9"/>
@@ -5497,256 +5555,266 @@
     <hyperlink ref="G2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="42.140625" customWidth="1"/>
+    <col min="2" max="2" width="42.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="24"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2" t="s">
+    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="4" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B40" s="4" t="s">
         <v>51</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -5760,7 +5828,7 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>